<commit_message>
Update Sprint Task Sheet - Team Hyrda.xlsx
</commit_message>
<xml_diff>
--- a/ProjectJournal/Sprint Task Sheet - Team Hyrda.xlsx
+++ b/ProjectJournal/Sprint Task Sheet - Team Hyrda.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anand\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeamHydra_Starbucks\ProjectJournal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD08E8D3-050C-4329-9346-E768795FCF63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875F3232-35A8-4007-BFB7-7695C2278CF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,18 +141,6 @@
     <t>Chaitrali + Prathyusha</t>
   </si>
   <si>
-    <t>Authentication</t>
-  </si>
-  <si>
-    <t>Add Cards</t>
-  </si>
-  <si>
-    <t>Managed Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payments </t>
-  </si>
-  <si>
     <t>Demo Presentations</t>
   </si>
   <si>
@@ -169,6 +157,18 @@
   </si>
   <si>
     <t>20 hours / Week</t>
+  </si>
+  <si>
+    <t>Payments and Store API</t>
+  </si>
+  <si>
+    <t>Managed Order API</t>
+  </si>
+  <si>
+    <t>Add Cards API</t>
+  </si>
+  <si>
+    <t>Authentication API</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1329,7 @@
   <dimension ref="A1:T1002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1376,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
@@ -1592,7 +1592,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>34</v>
@@ -1646,7 +1646,7 @@
     <row r="7" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>34</v>
@@ -1700,7 +1700,7 @@
     <row r="8" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="29" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>32</v>
@@ -1754,7 +1754,7 @@
     <row r="9" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>32</v>
@@ -1808,7 +1808,7 @@
     <row r="10" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
       <c r="B10" s="29" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>33</v>
@@ -1862,7 +1862,7 @@
     <row r="11" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>33</v>
@@ -1916,7 +1916,7 @@
     <row r="12" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="29" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>31</v>
@@ -1972,7 +1972,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>31</v>
@@ -2026,7 +2026,7 @@
     <row r="14" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>35</v>
@@ -2080,7 +2080,7 @@
     <row r="15" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>36</v>
@@ -2180,7 +2180,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
@@ -2206,7 +2206,7 @@
         <v>23</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -2232,7 +2232,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
@@ -2258,7 +2258,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>

</xml_diff>

<commit_message>
Added images for Burndown chart
</commit_message>
<xml_diff>
--- a/ProjectJournal/Sprint Task Sheet - Team Hyrda.xlsx
+++ b/ProjectJournal/Sprint Task Sheet - Team Hyrda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeamHydra_Starbucks\ProjectJournal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBB33CF-6D0A-419B-9E77-F222517145C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56143338-881A-424E-B5B4-4F09B13E6AA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint" sheetId="1" r:id="rId1"/>
@@ -577,7 +577,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Burndown (Team XXX)</a:t>
+              <a:t>Burndown (Team Hydra)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1310,7 +1310,7 @@
   </sheetPr>
   <dimension ref="A1:T1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -21915,8 +21915,8 @@
   </sheetPr>
   <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>